<commit_message>
Window size and email fix
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/QA_538.xlsx
+++ b/binaries/FCfiles/QA_538.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="93">
   <si>
     <t>serviceLevel</t>
   </si>
@@ -286,6 +286,21 @@
   </si>
   <si>
     <t>51499703</t>
+  </si>
+  <si>
+    <t>51500043</t>
+  </si>
+  <si>
+    <t>51500044</t>
+  </si>
+  <si>
+    <t>10-16-2021</t>
+  </si>
+  <si>
+    <t>51500047</t>
+  </si>
+  <si>
+    <t>51500054</t>
   </si>
 </sst>
 </file>
@@ -308,7 +323,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="59">
+  <fills count="73">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -600,8 +615,78 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="59">
+  <borders count="73">
     <border>
       <left/>
       <right/>
@@ -865,11 +950,60 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="42">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
@@ -904,7 +1038,14 @@
     <xf applyBorder="true" applyFill="true" borderId="52" fillId="52" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="54" fillId="54" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="56" fillId="56" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="58" borderId="58" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="58" fillId="58" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="60" fillId="60" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="62" fillId="62" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="64" fillId="64" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="66" fillId="66" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="68" fillId="68" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="70" fillId="70" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="72" borderId="72" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -1422,8 +1563,8 @@
       <c r="P2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Q2" s="29" t="s">
-        <v>83</v>
+      <c r="Q2" s="36" t="s">
+        <v>88</v>
       </c>
       <c r="R2" s="7"/>
       <c r="S2" s="1" t="s">
@@ -1506,11 +1647,11 @@
       <c r="P3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="R3" s="33" t="s">
-        <v>86</v>
+      <c r="Q3" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="R3" s="40" t="s">
+        <v>91</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>31</v>
@@ -1537,8 +1678,8 @@
       <c r="AC3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AD3" s="31" t="s">
-        <v>85</v>
+      <c r="AD3" s="38" t="s">
+        <v>90</v>
       </c>
       <c r="AE3" s="1" t="s">
         <v>56</v>
@@ -1592,8 +1733,8 @@
       <c r="P4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Q4" s="34" t="s">
-        <v>87</v>
+      <c r="Q4" s="41" t="s">
+        <v>92</v>
       </c>
       <c r="R4" s="5"/>
       <c r="S4" s="1" t="s">

</xml_diff>

<commit_message>
Email message screenshot addition
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/QA_538.xlsx
+++ b/binaries/FCfiles/QA_538.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="94">
   <si>
     <t>serviceLevel</t>
   </si>
@@ -301,6 +301,9 @@
   </si>
   <si>
     <t>51500054</t>
+  </si>
+  <si>
+    <t>51500206</t>
   </si>
 </sst>
 </file>
@@ -323,7 +326,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="73">
+  <fills count="75">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -685,8 +688,18 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="73">
+  <borders count="75">
     <border>
       <left/>
       <right/>
@@ -999,11 +1012,18 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
@@ -1045,7 +1065,8 @@
     <xf applyBorder="true" applyFill="true" borderId="66" fillId="66" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="68" fillId="68" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="70" fillId="70" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="72" borderId="72" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="72" fillId="72" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="74" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -1733,8 +1754,8 @@
       <c r="P4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Q4" s="41" t="s">
-        <v>92</v>
+      <c r="Q4" s="42" t="s">
+        <v>93</v>
       </c>
       <c r="R4" s="5"/>
       <c r="S4" s="1" t="s">

</xml_diff>